<commit_message>
look for nonzero entries for activitycode when importing pointsource, even when codesets do not exist
</commit_message>
<xml_diff>
--- a/tests/edb/data/pointsources.xlsx
+++ b/tests/edb/data/pointsources.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">activitycode_code_set2</t>
   </si>
   <si>
-    <t xml:space="preserve">Activitycode_3</t>
+    <t xml:space="preserve">activitycode_3</t>
   </si>
   <si>
     <t xml:space="preserve">chimney_height</t>
@@ -237,10 +237,10 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>